<commit_message>
🔧 update with model information
</commit_message>
<xml_diff>
--- a/static/template/Internal Statistical Reporting Template.xlsx
+++ b/static/template/Internal Statistical Reporting Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\var\neuralNOD\Core Neural Network (private)\static\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4173A67-0285-444E-8AAC-253DF5C2C71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76428000-2512-41E6-B11B-CBCDB7194964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{A8FA6C65-F4C8-40D2-818C-9F680934BC5F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A8FA6C65-F4C8-40D2-818C-9F680934BC5F}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>👾 &lt; neuralNOD /&gt;</t>
-  </si>
   <si>
     <t>AI Powered Engine to Forecast Market Clearing Price (MCP)</t>
   </si>
@@ -113,12 +110,37 @@
       <t>(internal reports - for training and validation)</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">👾 &lt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="22"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Ink Free"/>
+        <family val="4"/>
+      </rPr>
+      <t>neuralNOD</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Ink Free"/>
+        <family val="4"/>
+      </rPr>
+      <t xml:space="preserve"> /&gt;</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +231,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Ink Free"/>
+      <family val="4"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -230,7 +259,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -441,11 +470,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -468,6 +534,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -505,33 +607,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -861,32 +936,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="A1" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
       <c r="G3" s="2"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -897,45 +972,45 @@
       <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="10" t="s">
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="23"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="13"/>
       <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -946,122 +1021,122 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="21" t="s">
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="2"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="10" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="2"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="20" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="10" t="s">
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="10" t="s">
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="2"/>
-    </row>
-    <row r="10" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="10" t="s">
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="13"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="25"/>
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="16"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="28"/>
       <c r="O11" s="2"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -1081,39 +1156,39 @@
       <c r="N12" s="6"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
+      <c r="A13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
       <c r="O13" s="2"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
       <c r="O14" s="2"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -1125,36 +1200,37 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="A13:N14"/>
-    <mergeCell ref="H10:J11"/>
-    <mergeCell ref="K10:N11"/>
-    <mergeCell ref="C9:F11"/>
+  <mergeCells count="22">
+    <mergeCell ref="A1:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:F8"/>
     <mergeCell ref="H4:N4"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="A1:F4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="A9:B11"/>
+    <mergeCell ref="I15:N15"/>
     <mergeCell ref="K5:N5"/>
     <mergeCell ref="K6:N6"/>
     <mergeCell ref="K7:N7"/>
     <mergeCell ref="K8:N8"/>
     <mergeCell ref="K9:N9"/>
+    <mergeCell ref="A13:N14"/>
+    <mergeCell ref="H10:J11"/>
+    <mergeCell ref="K10:N11"/>
+    <mergeCell ref="C9:F11"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="A9:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>